<commit_message>
convert plotting notebook to scripts
</commit_message>
<xml_diff>
--- a/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
+++ b/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -227,7 +227,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +294,18 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -307,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,6 +346,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q98"/>
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P82" sqref="P82"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S74" sqref="S74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -695,11 +712,11 @@
     <col min="2" max="2" width="7.375" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="19.125" customWidth="1"/>
-    <col min="9" max="9" width="18.125" customWidth="1"/>
-    <col min="10" max="10" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="16.875" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="79.125" customWidth="1"/>
@@ -1379,8 +1396,6 @@
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1419,8 +1434,6 @@
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
       <c r="Q18" s="22"/>
     </row>
     <row r="19" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1459,8 +1472,6 @@
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
       <c r="Q19" s="23"/>
     </row>
     <row r="20" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1503,8 +1514,6 @@
       <c r="M20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
       <c r="Q20" s="23"/>
     </row>
     <row r="21" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1545,8 +1554,6 @@
         <v>49</v>
       </c>
       <c r="M21" s="7"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
       <c r="Q21" s="23"/>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1587,8 +1594,6 @@
         <v>7</v>
       </c>
       <c r="M22" s="7"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
       <c r="Q22" s="23"/>
     </row>
     <row r="23" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2668,7 +2673,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>21</v>
       </c>
@@ -2705,7 +2710,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -2742,7 +2747,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>21</v>
       </c>
@@ -2779,7 +2784,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>21</v>
       </c>
@@ -2817,8 +2822,14 @@
         <v>50</v>
       </c>
       <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O52" t="s">
+        <v>22</v>
+      </c>
+      <c r="P52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>21</v>
       </c>
@@ -2858,8 +2869,14 @@
       <c r="M53" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O53" s="22">
+        <v>51</v>
+      </c>
+      <c r="P53" s="22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>21</v>
       </c>
@@ -2899,8 +2916,14 @@
       <c r="M54" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O54" s="22">
+        <v>62</v>
+      </c>
+      <c r="P54" s="22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>21</v>
       </c>
@@ -2938,8 +2961,14 @@
         <v>55</v>
       </c>
       <c r="M55" s="7"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O55" s="22">
+        <v>94</v>
+      </c>
+      <c r="P55" s="22">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>21</v>
       </c>
@@ -2977,8 +3006,20 @@
         <v>44</v>
       </c>
       <c r="M56" s="7"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O56" s="3">
+        <v>106</v>
+      </c>
+      <c r="P56" s="3">
+        <v>11</v>
+      </c>
+      <c r="R56" s="7">
+        <v>67</v>
+      </c>
+      <c r="S56" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -3014,8 +3055,20 @@
       </c>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>67</v>
+      </c>
+      <c r="P57">
+        <v>13</v>
+      </c>
+      <c r="R57" s="7">
+        <v>100</v>
+      </c>
+      <c r="S57" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>21</v>
       </c>
@@ -3051,8 +3104,14 @@
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>100</v>
+      </c>
+      <c r="P58">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>21</v>
       </c>
@@ -3088,8 +3147,14 @@
       </c>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>83</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>21</v>
       </c>
@@ -3129,8 +3194,14 @@
       <c r="M60" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>72</v>
+      </c>
+      <c r="P60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>21</v>
       </c>
@@ -3166,8 +3237,14 @@
       </c>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>78</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>21</v>
       </c>
@@ -3203,8 +3280,14 @@
       </c>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O62" s="7">
+        <v>78</v>
+      </c>
+      <c r="P62" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>21</v>
       </c>
@@ -3240,8 +3323,14 @@
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O63" s="11">
+        <v>94</v>
+      </c>
+      <c r="P63" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>21</v>
       </c>
@@ -3277,83 +3366,95 @@
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
+      <c r="O64" s="7">
+        <v>66</v>
+      </c>
+      <c r="P64" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="15">
+      <c r="A65" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="28">
         <v>23</v>
       </c>
-      <c r="C65" s="15">
+      <c r="C65" s="28">
         <v>211104</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="15">
-        <v>1</v>
-      </c>
-      <c r="F65" s="15">
-        <v>0</v>
-      </c>
-      <c r="G65" s="15">
-        <v>0</v>
-      </c>
-      <c r="H65" s="15">
-        <v>0</v>
-      </c>
-      <c r="I65" s="15">
-        <v>0</v>
-      </c>
-      <c r="J65" s="15">
-        <v>0</v>
-      </c>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
+      <c r="D65" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="28">
+        <v>1</v>
+      </c>
+      <c r="F65" s="28">
+        <v>0</v>
+      </c>
+      <c r="G65" s="28">
+        <v>0</v>
+      </c>
+      <c r="H65" s="28">
+        <v>0</v>
+      </c>
+      <c r="I65" s="28">
+        <v>0</v>
+      </c>
+      <c r="J65" s="28">
+        <v>0</v>
+      </c>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="O65" s="7">
+        <v>68</v>
+      </c>
+      <c r="P65" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="18">
+      <c r="A66" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="26">
         <v>23</v>
       </c>
-      <c r="C66" s="18">
+      <c r="C66" s="26">
         <v>211104</v>
       </c>
-      <c r="D66" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E66" s="20">
-        <v>1</v>
-      </c>
-      <c r="F66" s="20">
-        <v>0</v>
-      </c>
-      <c r="G66" s="20">
-        <v>0</v>
-      </c>
-      <c r="H66" s="20">
-        <v>0</v>
-      </c>
-      <c r="I66" s="20">
-        <v>0</v>
-      </c>
-      <c r="J66" s="20">
-        <v>0</v>
-      </c>
-      <c r="K66" s="20"/>
-      <c r="L66" s="20"/>
-      <c r="M66" s="20" t="s">
+      <c r="D66" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="28">
+        <v>1</v>
+      </c>
+      <c r="F66" s="28">
+        <v>0</v>
+      </c>
+      <c r="G66" s="28">
+        <v>0</v>
+      </c>
+      <c r="H66" s="28">
+        <v>0</v>
+      </c>
+      <c r="I66" s="28">
+        <v>0</v>
+      </c>
+      <c r="J66" s="28">
+        <v>0</v>
+      </c>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="O66" t="s">
-        <v>22</v>
-      </c>
-      <c r="P66" t="s">
-        <v>24</v>
+      <c r="O66">
+        <v>53</v>
+      </c>
+      <c r="P66">
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3392,8 +3493,12 @@
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
-      <c r="O67" s="22"/>
-      <c r="P67" s="22"/>
+      <c r="O67">
+        <v>109</v>
+      </c>
+      <c r="P67">
+        <v>67</v>
+      </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
@@ -3431,84 +3536,96 @@
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="22"/>
+      <c r="O68">
+        <v>126</v>
+      </c>
+      <c r="P68">
+        <v>38</v>
+      </c>
       <c r="Q68" s="22"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" s="13">
+      <c r="A69" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="26">
         <v>23</v>
       </c>
-      <c r="C69" s="13">
+      <c r="C69" s="26">
         <v>211105</v>
       </c>
-      <c r="D69" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E69" s="15">
-        <v>1</v>
-      </c>
-      <c r="F69" s="15">
-        <v>0</v>
-      </c>
-      <c r="G69" s="15">
-        <v>0</v>
-      </c>
-      <c r="H69" s="15">
-        <v>0</v>
-      </c>
-      <c r="I69" s="15">
-        <v>0</v>
-      </c>
-      <c r="J69" s="15">
-        <v>0</v>
-      </c>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="O69" s="22"/>
-      <c r="P69" s="22"/>
+      <c r="D69" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" s="28">
+        <v>1</v>
+      </c>
+      <c r="F69" s="28">
+        <v>0</v>
+      </c>
+      <c r="G69" s="28">
+        <v>0</v>
+      </c>
+      <c r="H69" s="28">
+        <v>0</v>
+      </c>
+      <c r="I69" s="28">
+        <v>0</v>
+      </c>
+      <c r="J69" s="28">
+        <v>0</v>
+      </c>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="O69" s="3">
+        <v>97</v>
+      </c>
+      <c r="P69" s="3">
+        <v>33</v>
+      </c>
       <c r="Q69" s="22"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B70" s="13">
+      <c r="A70" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="26">
         <v>23</v>
       </c>
-      <c r="C70" s="13">
+      <c r="C70" s="26">
         <v>211105</v>
       </c>
-      <c r="D70" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="15">
-        <v>1</v>
-      </c>
-      <c r="F70" s="15">
-        <v>0</v>
-      </c>
-      <c r="G70" s="15">
-        <v>0</v>
-      </c>
-      <c r="H70" s="15">
-        <v>0</v>
-      </c>
-      <c r="I70" s="15">
-        <v>0</v>
-      </c>
-      <c r="J70" s="15">
-        <v>0</v>
-      </c>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="O70" s="22"/>
-      <c r="P70" s="22"/>
+      <c r="D70" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="28">
+        <v>1</v>
+      </c>
+      <c r="F70" s="28">
+        <v>0</v>
+      </c>
+      <c r="G70" s="28">
+        <v>0</v>
+      </c>
+      <c r="H70" s="28">
+        <v>0</v>
+      </c>
+      <c r="I70" s="28">
+        <v>0</v>
+      </c>
+      <c r="J70" s="28">
+        <v>0</v>
+      </c>
+      <c r="K70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="28"/>
+      <c r="O70">
+        <v>98</v>
+      </c>
+      <c r="P70">
+        <v>41</v>
+      </c>
       <c r="Q70" s="22"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -3549,8 +3666,12 @@
       <c r="M71" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="O71" s="22"/>
-      <c r="P71" s="22"/>
+      <c r="O71">
+        <v>99</v>
+      </c>
+      <c r="P71">
+        <v>36</v>
+      </c>
       <c r="Q71" s="22"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -3589,8 +3710,12 @@
       </c>
       <c r="L72" s="12"/>
       <c r="M72" s="12"/>
-      <c r="O72" s="22"/>
-      <c r="P72" s="22"/>
+      <c r="O72">
+        <v>168</v>
+      </c>
+      <c r="P72">
+        <v>55</v>
+      </c>
       <c r="Q72" s="22"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -3629,8 +3754,12 @@
       </c>
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
-      <c r="O73" s="22"/>
-      <c r="P73" s="22"/>
+      <c r="O73">
+        <v>139</v>
+      </c>
+      <c r="P73">
+        <v>24</v>
+      </c>
       <c r="Q73" s="22"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -3670,12 +3799,10 @@
       <c r="L74" s="15"/>
       <c r="M74" s="15"/>
       <c r="O74">
-        <f>SUM(O67:O73)</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="P74">
-        <f>SUM(P67:P73)</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="Q74" s="22"/>
     </row>
@@ -3716,12 +3843,10 @@
         <v>57</v>
       </c>
       <c r="O75">
-        <f>0.7*O74</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="P75">
-        <f>0.7*P74</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="Q75" s="22"/>
     </row>
@@ -3761,6 +3886,12 @@
       <c r="M76" s="20" t="s">
         <v>56</v>
       </c>
+      <c r="O76" s="22">
+        <v>98</v>
+      </c>
+      <c r="P76" s="22">
+        <v>42</v>
+      </c>
       <c r="Q76" s="22"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -3799,6 +3930,12 @@
       </c>
       <c r="L77" s="15"/>
       <c r="M77" s="15"/>
+      <c r="O77" s="22">
+        <v>52</v>
+      </c>
+      <c r="P77" s="22">
+        <v>47</v>
+      </c>
       <c r="Q77" s="22"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -3837,78 +3974,96 @@
       </c>
       <c r="L78" s="15"/>
       <c r="M78" s="15"/>
+      <c r="O78" s="22">
+        <v>79</v>
+      </c>
+      <c r="P78" s="22">
+        <v>58</v>
+      </c>
       <c r="Q78" s="22"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B79" s="13">
+      <c r="A79" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="26">
         <v>23</v>
       </c>
-      <c r="C79" s="13">
+      <c r="C79" s="26">
         <v>211109</v>
       </c>
-      <c r="D79" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="15">
-        <v>1</v>
-      </c>
-      <c r="F79" s="15">
-        <v>0</v>
-      </c>
-      <c r="G79" s="15">
-        <v>0</v>
-      </c>
-      <c r="H79" s="15">
-        <v>0</v>
-      </c>
-      <c r="I79" s="15">
-        <v>0</v>
-      </c>
-      <c r="J79" s="15">
-        <v>0</v>
-      </c>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
+      <c r="D79" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="28">
+        <v>1</v>
+      </c>
+      <c r="F79" s="28">
+        <v>0</v>
+      </c>
+      <c r="G79" s="28">
+        <v>0</v>
+      </c>
+      <c r="H79" s="28">
+        <v>0</v>
+      </c>
+      <c r="I79" s="28">
+        <v>0</v>
+      </c>
+      <c r="J79" s="28">
+        <v>0</v>
+      </c>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="28"/>
+      <c r="O79" s="22">
+        <v>60</v>
+      </c>
+      <c r="P79" s="22">
+        <v>35</v>
+      </c>
       <c r="Q79" s="22"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B80" s="13">
+      <c r="A80" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="26">
         <v>23</v>
       </c>
-      <c r="C80" s="13">
+      <c r="C80" s="26">
         <v>211109</v>
       </c>
-      <c r="D80" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E80" s="15">
-        <v>1</v>
-      </c>
-      <c r="F80" s="15">
-        <v>0</v>
-      </c>
-      <c r="G80" s="15">
-        <v>0</v>
-      </c>
-      <c r="H80" s="15">
-        <v>0</v>
-      </c>
-      <c r="I80" s="15">
-        <v>0</v>
-      </c>
-      <c r="J80" s="15">
-        <v>0</v>
-      </c>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
+      <c r="D80" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="28">
+        <v>1</v>
+      </c>
+      <c r="F80" s="28">
+        <v>0</v>
+      </c>
+      <c r="G80" s="28">
+        <v>0</v>
+      </c>
+      <c r="H80" s="28">
+        <v>0</v>
+      </c>
+      <c r="I80" s="28">
+        <v>0</v>
+      </c>
+      <c r="J80" s="28">
+        <v>0</v>
+      </c>
+      <c r="K80" s="28"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="28"/>
+      <c r="O80" s="22">
+        <v>38</v>
+      </c>
+      <c r="P80" s="22">
+        <v>0</v>
+      </c>
       <c r="Q80" s="22"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -3947,6 +4102,12 @@
       </c>
       <c r="L81" s="15"/>
       <c r="M81" s="15"/>
+      <c r="O81" s="22">
+        <v>79</v>
+      </c>
+      <c r="P81" s="22">
+        <v>34</v>
+      </c>
       <c r="Q81" s="22"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -3985,6 +4146,12 @@
       </c>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
+      <c r="O82" s="22">
+        <v>62</v>
+      </c>
+      <c r="P82" s="22">
+        <v>97</v>
+      </c>
       <c r="Q82" s="22"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
@@ -4018,11 +4185,19 @@
       <c r="J83" s="15">
         <v>0</v>
       </c>
-      <c r="K83" s="15"/>
+      <c r="K83" s="15">
+        <v>19</v>
+      </c>
       <c r="L83" s="15"/>
       <c r="M83" s="15" t="s">
         <v>55</v>
       </c>
+      <c r="O83">
+        <v>79</v>
+      </c>
+      <c r="P83">
+        <v>101</v>
+      </c>
       <c r="Q83" s="22"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -4056,9 +4231,17 @@
       <c r="J84" s="15">
         <v>0</v>
       </c>
-      <c r="K84" s="15"/>
+      <c r="K84" s="15">
+        <v>39</v>
+      </c>
       <c r="L84" s="15"/>
       <c r="M84" s="15"/>
+      <c r="O84">
+        <v>59</v>
+      </c>
+      <c r="P84">
+        <v>109</v>
+      </c>
       <c r="Q84" s="22"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
@@ -4092,11 +4275,19 @@
       <c r="J85" s="15">
         <v>0</v>
       </c>
-      <c r="K85" s="15"/>
+      <c r="K85" s="15">
+        <v>102</v>
+      </c>
       <c r="L85" s="15"/>
       <c r="M85" s="15" t="s">
         <v>55</v>
       </c>
+      <c r="O85">
+        <v>75</v>
+      </c>
+      <c r="P85">
+        <v>84</v>
+      </c>
       <c r="Q85" s="22"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
@@ -4130,9 +4321,17 @@
       <c r="J86" s="15">
         <v>0</v>
       </c>
-      <c r="K86" s="15"/>
+      <c r="K86" s="15">
+        <v>49</v>
+      </c>
       <c r="L86" s="15"/>
       <c r="M86" s="15"/>
+      <c r="O86">
+        <v>166</v>
+      </c>
+      <c r="P86">
+        <v>52</v>
+      </c>
       <c r="Q86" s="22"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
@@ -4166,11 +4365,19 @@
       <c r="J87" s="15">
         <v>0</v>
       </c>
-      <c r="K87" s="15"/>
+      <c r="K87" s="15">
+        <v>136</v>
+      </c>
       <c r="L87" s="15"/>
       <c r="M87" s="15" t="s">
         <v>55</v>
       </c>
+      <c r="O87">
+        <v>140</v>
+      </c>
+      <c r="P87">
+        <v>105</v>
+      </c>
       <c r="Q87" s="22"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -4204,9 +4411,17 @@
       <c r="J88" s="15">
         <v>0</v>
       </c>
-      <c r="K88" s="15"/>
+      <c r="K88" s="15">
+        <v>68</v>
+      </c>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
+      <c r="O88">
+        <v>19</v>
+      </c>
+      <c r="P88">
+        <v>39</v>
+      </c>
       <c r="Q88" s="22"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -4245,6 +4460,12 @@
       </c>
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
+      <c r="O89">
+        <v>102</v>
+      </c>
+      <c r="P89">
+        <v>49</v>
+      </c>
       <c r="Q89" s="22"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -4283,268 +4504,470 @@
       </c>
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
+      <c r="O90">
+        <v>136</v>
+      </c>
+      <c r="P90">
+        <v>68</v>
+      </c>
       <c r="Q90" s="22"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A91" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B91" s="21">
+      <c r="A91" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="24">
         <v>28</v>
       </c>
-      <c r="C91" s="21">
+      <c r="C91" s="24">
         <v>211115</v>
       </c>
-      <c r="D91" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91">
-        <v>0</v>
-      </c>
-      <c r="J91">
-        <v>0</v>
+      <c r="D91" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" s="15">
+        <v>0</v>
+      </c>
+      <c r="F91" s="15">
+        <v>0</v>
+      </c>
+      <c r="G91" s="15">
+        <v>0</v>
+      </c>
+      <c r="H91" s="15">
+        <v>0</v>
+      </c>
+      <c r="I91" s="15">
+        <v>0</v>
+      </c>
+      <c r="J91" s="15">
+        <v>0</v>
+      </c>
+      <c r="K91" s="15">
+        <v>94</v>
+      </c>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
+      <c r="O91">
+        <v>76</v>
+      </c>
+      <c r="P91">
+        <v>100</v>
       </c>
       <c r="Q91" s="22"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B92" s="21">
+      <c r="A92" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" s="24">
         <v>28</v>
       </c>
-      <c r="C92" s="21">
+      <c r="C92" s="24">
         <v>211115</v>
       </c>
-      <c r="D92" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92">
-        <v>0</v>
-      </c>
-      <c r="J92">
-        <v>0</v>
+      <c r="D92" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" s="15">
+        <v>0</v>
+      </c>
+      <c r="F92" s="15">
+        <v>0</v>
+      </c>
+      <c r="G92" s="15">
+        <v>0</v>
+      </c>
+      <c r="H92" s="15">
+        <v>0</v>
+      </c>
+      <c r="I92" s="15">
+        <v>0</v>
+      </c>
+      <c r="J92" s="15">
+        <v>0</v>
+      </c>
+      <c r="K92" s="15">
+        <v>62</v>
+      </c>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="O92">
+        <v>94</v>
+      </c>
+      <c r="P92">
+        <v>62</v>
       </c>
       <c r="Q92" s="22"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B93" s="21">
+      <c r="A93" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="24">
         <v>28</v>
       </c>
-      <c r="C93" s="21">
+      <c r="C93" s="24">
         <v>211116</v>
       </c>
-      <c r="D93" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-      <c r="H93">
-        <v>0</v>
-      </c>
-      <c r="I93">
-        <v>0</v>
-      </c>
-      <c r="J93">
-        <v>0</v>
+      <c r="D93" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="15">
+        <v>0</v>
+      </c>
+      <c r="F93" s="15">
+        <v>0</v>
+      </c>
+      <c r="G93" s="15">
+        <v>0</v>
+      </c>
+      <c r="H93" s="15">
+        <v>0</v>
+      </c>
+      <c r="I93" s="15">
+        <v>0</v>
+      </c>
+      <c r="J93" s="15">
+        <v>0</v>
+      </c>
+      <c r="K93" s="15">
+        <v>126</v>
+      </c>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="O93">
+        <v>126</v>
+      </c>
+      <c r="P93">
+        <v>64</v>
       </c>
       <c r="Q93" s="22"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="21">
+      <c r="A94" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" s="24">
         <v>28</v>
       </c>
-      <c r="C94" s="21">
+      <c r="C94" s="24">
         <v>211116</v>
       </c>
-      <c r="D94" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94">
-        <v>0</v>
-      </c>
-      <c r="J94">
-        <v>0</v>
+      <c r="D94" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="15">
+        <v>0</v>
+      </c>
+      <c r="F94" s="15">
+        <v>0</v>
+      </c>
+      <c r="G94" s="15">
+        <v>0</v>
+      </c>
+      <c r="H94" s="15">
+        <v>0</v>
+      </c>
+      <c r="I94" s="15">
+        <v>0</v>
+      </c>
+      <c r="J94" s="15">
+        <v>0</v>
+      </c>
+      <c r="K94" s="15">
+        <v>64</v>
+      </c>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="O94">
+        <v>78</v>
+      </c>
+      <c r="P94">
+        <v>84</v>
       </c>
       <c r="Q94" s="22"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A95" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B95" s="21">
+      <c r="A95" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" s="24">
         <v>29</v>
       </c>
-      <c r="C95" s="21">
+      <c r="C95" s="24">
         <v>211116</v>
       </c>
-      <c r="D95" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95">
-        <v>0</v>
-      </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95">
-        <v>0</v>
-      </c>
-      <c r="J95">
-        <v>0</v>
+      <c r="D95" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="15">
+        <v>0</v>
+      </c>
+      <c r="F95" s="15">
+        <v>0</v>
+      </c>
+      <c r="G95" s="15">
+        <v>0</v>
+      </c>
+      <c r="H95" s="15">
+        <v>0</v>
+      </c>
+      <c r="I95" s="15">
+        <v>0</v>
+      </c>
+      <c r="J95" s="15">
+        <v>0</v>
+      </c>
+      <c r="K95" s="15">
+        <v>78</v>
+      </c>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="O95">
+        <v>88</v>
+      </c>
+      <c r="P95">
+        <v>131</v>
       </c>
       <c r="Q95" s="22"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B96" s="21">
+      <c r="A96" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" s="24">
         <v>29</v>
       </c>
-      <c r="C96" s="21">
+      <c r="C96" s="24">
         <v>211116</v>
       </c>
-      <c r="D96" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96">
-        <v>0</v>
-      </c>
-      <c r="J96">
-        <v>0</v>
+      <c r="D96" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0</v>
+      </c>
+      <c r="F96" s="15">
+        <v>0</v>
+      </c>
+      <c r="G96" s="15">
+        <v>0</v>
+      </c>
+      <c r="H96" s="15">
+        <v>0</v>
+      </c>
+      <c r="I96" s="15">
+        <v>0</v>
+      </c>
+      <c r="J96" s="15">
+        <v>0</v>
+      </c>
+      <c r="K96" s="15">
+        <v>84</v>
+      </c>
+      <c r="L96" s="15"/>
+      <c r="M96" s="15"/>
+      <c r="O96">
+        <v>98</v>
+      </c>
+      <c r="P96">
+        <v>68</v>
       </c>
       <c r="Q96" s="22"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B97" s="21">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="24">
         <v>28</v>
       </c>
-      <c r="C97" s="21">
+      <c r="C97" s="24">
         <v>211117</v>
       </c>
-      <c r="D97" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
-      </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97">
-        <v>0</v>
-      </c>
-      <c r="I97">
-        <v>0</v>
-      </c>
-      <c r="J97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="21">
+      <c r="D97" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" s="15">
+        <v>0</v>
+      </c>
+      <c r="F97" s="15">
+        <v>0</v>
+      </c>
+      <c r="G97" s="15">
+        <v>0</v>
+      </c>
+      <c r="H97" s="15">
+        <v>0</v>
+      </c>
+      <c r="I97" s="15">
+        <v>0</v>
+      </c>
+      <c r="J97" s="15">
+        <v>0</v>
+      </c>
+      <c r="K97" s="15">
+        <v>88</v>
+      </c>
+      <c r="L97" s="15"/>
+      <c r="M97" s="15"/>
+      <c r="O97">
+        <v>127</v>
+      </c>
+      <c r="P97">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="24">
         <v>28</v>
       </c>
-      <c r="C98" s="21">
+      <c r="C98" s="24">
         <v>211117</v>
       </c>
-      <c r="D98" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-      <c r="I98">
-        <v>0</v>
-      </c>
-      <c r="J98">
-        <v>0</v>
+      <c r="D98" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0</v>
+      </c>
+      <c r="F98" s="15">
+        <v>0</v>
+      </c>
+      <c r="G98" s="15">
+        <v>0</v>
+      </c>
+      <c r="H98" s="15">
+        <v>0</v>
+      </c>
+      <c r="I98" s="15">
+        <v>0</v>
+      </c>
+      <c r="J98" s="15">
+        <v>0</v>
+      </c>
+      <c r="K98" s="15">
+        <v>131</v>
+      </c>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="O98">
+        <f>SUM(O53:O97)</f>
+        <v>3974</v>
+      </c>
+      <c r="P98">
+        <f>SUM(P53:P97)</f>
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A99" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="24">
+        <v>28</v>
+      </c>
+      <c r="C99" s="24">
+        <v>211118</v>
+      </c>
+      <c r="D99" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15">
+        <v>98</v>
+      </c>
+      <c r="L99" s="15"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="O99">
+        <f>0.7*O98</f>
+        <v>2781.7999999999997</v>
+      </c>
+      <c r="P99">
+        <f>0.7*P98</f>
+        <v>1535.8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A100" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="24">
+        <v>28</v>
+      </c>
+      <c r="C100" s="24">
+        <v>211118</v>
+      </c>
+      <c r="D100" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15">
+        <v>68</v>
+      </c>
+      <c r="L100" s="15"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="O100">
+        <f>0.6*O98</f>
+        <v>2384.4</v>
+      </c>
+      <c r="P100">
+        <f>0.6*P98</f>
+        <v>1316.3999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A101" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" s="24">
+        <v>29</v>
+      </c>
+      <c r="C101" s="24">
+        <v>211118</v>
+      </c>
+      <c r="D101" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K101" s="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A102" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="24">
+        <v>29</v>
+      </c>
+      <c r="C102" s="24">
+        <v>211118</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K102" s="15">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update docs and notes
</commit_message>
<xml_diff>
--- a/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
+++ b/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>CUDA error but might just be from PFC, need to check</t>
+  </si>
+  <si>
+    <t>a lot of the clusters were noise/purely contamination, lower spike count, 1 cluster excluded</t>
+  </si>
+  <si>
+    <t>exclude unless desparately need data</t>
+  </si>
+  <si>
+    <t>noise in signal from turning off manipulator controller? Check that brain regions and channel mapping are correct too</t>
+  </si>
+  <si>
+    <t>Recordings left to do:</t>
+  </si>
+  <si>
+    <t>there were at least 4 instances of double counting so I had to throw out a lot of the clusters with less than 1000 spikes</t>
+  </si>
+  <si>
+    <t>Transferred to my desktop for curation later - Steph</t>
   </si>
 </sst>
 </file>
@@ -227,7 +245,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +324,12 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,6 +375,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,11 +726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S102"/>
+  <dimension ref="A1:S119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S74" sqref="S74"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -712,11 +739,11 @@
     <col min="2" max="2" width="7.375" customWidth="1"/>
     <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="16" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="18.125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="20.125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
+    <col min="10" max="10" width="20.125" customWidth="1"/>
     <col min="11" max="11" width="16.875" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="79.125" customWidth="1"/>
@@ -1044,41 +1071,49 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="A9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="16">
         <v>17</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="16">
         <v>210410</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="D9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1</v>
+      </c>
+      <c r="K9" s="16">
         <v>62</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="L9" s="16">
+        <v>40</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1097,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -1115,7 +1150,9 @@
         <v>56</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
@@ -1137,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1155,7 +1192,9 @@
         <v>94</v>
       </c>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="22"/>
@@ -1177,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -1195,7 +1234,9 @@
         <v>68</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
@@ -1361,79 +1402,79 @@
       <c r="Q16" s="22"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="A17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="16">
         <v>17</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="16">
         <v>210415</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
+      <c r="D17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1</v>
+      </c>
+      <c r="I17" s="16">
+        <v>1</v>
+      </c>
+      <c r="J17" s="16">
+        <v>1</v>
+      </c>
+      <c r="K17" s="16">
         <v>100</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
       <c r="Q17" s="22"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16">
         <v>17</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="16">
         <v>210415</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>22</v>
-      </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="D18" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1</v>
+      </c>
+      <c r="G18" s="16">
+        <v>1</v>
+      </c>
+      <c r="H18" s="16">
+        <v>1</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1</v>
+      </c>
+      <c r="J18" s="16">
+        <v>1</v>
+      </c>
+      <c r="K18" s="16">
+        <v>22</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
       <c r="Q18" s="22"/>
     </row>
     <row r="19" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1503,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
@@ -1667,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="3">
         <v>0</v>
@@ -1753,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="3">
         <v>0</v>
@@ -1831,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="3">
         <v>0</v>
@@ -2028,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="4">
         <v>0</v>
@@ -2046,7 +2087,9 @@
         <v>109</v>
       </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N33" s="6">
         <v>10</v>
       </c>
@@ -2071,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="4">
         <v>0</v>
@@ -2089,7 +2132,9 @@
         <v>67</v>
       </c>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N34" s="8">
         <v>30</v>
       </c>
@@ -2445,10 +2490,10 @@
         <v>1</v>
       </c>
       <c r="I43" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="7">
         <v>168</v>
@@ -2492,10 +2537,10 @@
         <v>1</v>
       </c>
       <c r="I44" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="7">
         <v>55</v>
@@ -2512,41 +2557,43 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="4">
+      <c r="A45" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="16">
         <v>25</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="17">
         <v>210907</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="4">
-        <v>1</v>
-      </c>
-      <c r="F45" s="4">
-        <v>0</v>
-      </c>
-      <c r="G45" s="4">
-        <v>0</v>
-      </c>
-      <c r="H45" s="4">
-        <v>0</v>
-      </c>
-      <c r="I45" s="4">
-        <v>0</v>
-      </c>
-      <c r="J45" s="4">
-        <v>0</v>
-      </c>
-      <c r="K45" s="4">
+      <c r="D45" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="16">
+        <v>1</v>
+      </c>
+      <c r="F45" s="16">
+        <v>1</v>
+      </c>
+      <c r="G45" s="16">
+        <v>1</v>
+      </c>
+      <c r="H45" s="16">
+        <v>1</v>
+      </c>
+      <c r="I45" s="16">
+        <v>1</v>
+      </c>
+      <c r="J45" s="16">
+        <v>1</v>
+      </c>
+      <c r="K45" s="16">
         <v>139</v>
       </c>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
+      <c r="L45" s="16">
+        <v>91</v>
+      </c>
+      <c r="M45" s="16"/>
       <c r="N45">
         <f>N44*0.7</f>
         <v>639.79999999999995</v>
@@ -2556,41 +2603,43 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="4">
+      <c r="A46" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="16">
         <v>25</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="17">
         <v>210907</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="4">
-        <v>1</v>
-      </c>
-      <c r="F46" s="4">
-        <v>0</v>
-      </c>
-      <c r="G46" s="4">
-        <v>0</v>
-      </c>
-      <c r="H46" s="4">
-        <v>0</v>
-      </c>
-      <c r="I46" s="4">
-        <v>0</v>
-      </c>
-      <c r="J46" s="4">
-        <v>0</v>
-      </c>
-      <c r="K46" s="4">
-        <v>24</v>
-      </c>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="D46" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="16">
+        <v>1</v>
+      </c>
+      <c r="F46" s="16">
+        <v>1</v>
+      </c>
+      <c r="G46" s="16">
+        <v>1</v>
+      </c>
+      <c r="H46" s="16">
+        <v>1</v>
+      </c>
+      <c r="I46" s="16">
+        <v>1</v>
+      </c>
+      <c r="J46" s="16">
+        <v>1</v>
+      </c>
+      <c r="K46" s="16">
+        <v>24</v>
+      </c>
+      <c r="L46" s="16">
+        <v>22</v>
+      </c>
+      <c r="M46" s="16"/>
       <c r="N46">
         <f>N44*0.6</f>
         <v>548.4</v>
@@ -2952,7 +3001,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="7">
         <v>79</v>
@@ -3183,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60" s="3">
         <v>0</v>
@@ -3288,41 +3337,43 @@
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B63" s="13">
+      <c r="A63" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="29">
         <v>29</v>
       </c>
-      <c r="C63" s="13">
+      <c r="C63" s="29">
         <v>211104</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E63" s="15">
-        <v>1</v>
-      </c>
-      <c r="F63" s="15">
-        <v>0</v>
-      </c>
-      <c r="G63" s="15">
-        <v>0</v>
-      </c>
-      <c r="H63" s="15">
-        <v>0</v>
-      </c>
-      <c r="I63" s="15">
-        <v>0</v>
-      </c>
-      <c r="J63" s="15">
-        <v>0</v>
-      </c>
-      <c r="K63" s="15">
+      <c r="D63" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="30">
+        <v>1</v>
+      </c>
+      <c r="F63" s="30">
+        <v>1</v>
+      </c>
+      <c r="G63" s="30">
+        <v>1</v>
+      </c>
+      <c r="H63" s="30">
+        <v>1</v>
+      </c>
+      <c r="I63" s="30">
+        <v>1</v>
+      </c>
+      <c r="J63" s="30">
+        <v>1</v>
+      </c>
+      <c r="K63" s="30">
         <v>62</v>
       </c>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
+      <c r="L63" s="30">
+        <v>46</v>
+      </c>
+      <c r="M63" s="30"/>
       <c r="O63" s="11">
         <v>94</v>
       </c>
@@ -3331,41 +3382,43 @@
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64" s="13">
+      <c r="A64" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="29">
         <v>29</v>
       </c>
-      <c r="C64" s="13">
+      <c r="C64" s="29">
         <v>211104</v>
       </c>
-      <c r="D64" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E64" s="15">
-        <v>1</v>
-      </c>
-      <c r="F64" s="15">
-        <v>0</v>
-      </c>
-      <c r="G64" s="15">
-        <v>0</v>
-      </c>
-      <c r="H64" s="15">
-        <v>0</v>
-      </c>
-      <c r="I64" s="15">
-        <v>0</v>
-      </c>
-      <c r="J64" s="15">
-        <v>0</v>
-      </c>
-      <c r="K64" s="15">
+      <c r="D64" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="30">
+        <v>1</v>
+      </c>
+      <c r="F64" s="30">
+        <v>1</v>
+      </c>
+      <c r="G64" s="30">
+        <v>1</v>
+      </c>
+      <c r="H64" s="30">
+        <v>1</v>
+      </c>
+      <c r="I64" s="30">
+        <v>1</v>
+      </c>
+      <c r="J64" s="30">
+        <v>1</v>
+      </c>
+      <c r="K64" s="30">
         <v>97</v>
       </c>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
+      <c r="L64" s="30">
+        <v>70</v>
+      </c>
+      <c r="M64" s="30"/>
       <c r="O64" s="7">
         <v>66</v>
       </c>
@@ -3402,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65" s="28"/>
       <c r="L65" s="28"/>
@@ -3443,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="28"/>
       <c r="L66" s="28"/>
@@ -3458,41 +3511,43 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="13">
+      <c r="A67" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="29">
         <v>29</v>
       </c>
-      <c r="C67" s="13">
+      <c r="C67" s="29">
         <v>211105</v>
       </c>
-      <c r="D67" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="15">
-        <v>1</v>
-      </c>
-      <c r="F67" s="15">
-        <v>1</v>
-      </c>
-      <c r="G67" s="15">
-        <v>0</v>
-      </c>
-      <c r="H67" s="15">
-        <v>0</v>
-      </c>
-      <c r="I67" s="15">
-        <v>0</v>
-      </c>
-      <c r="J67" s="15">
-        <v>0</v>
-      </c>
-      <c r="K67" s="15">
+      <c r="D67" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="30">
+        <v>1</v>
+      </c>
+      <c r="F67" s="30">
+        <v>1</v>
+      </c>
+      <c r="G67" s="30">
+        <v>1</v>
+      </c>
+      <c r="H67" s="30">
+        <v>1</v>
+      </c>
+      <c r="I67" s="30">
+        <v>1</v>
+      </c>
+      <c r="J67" s="30">
+        <v>1</v>
+      </c>
+      <c r="K67" s="30">
         <v>79</v>
       </c>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
+      <c r="L67" s="30">
+        <v>53</v>
+      </c>
+      <c r="M67" s="30"/>
       <c r="O67">
         <v>109</v>
       </c>
@@ -3501,41 +3556,43 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" s="13">
+      <c r="A68" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="29">
         <v>29</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C68" s="29">
         <v>211105</v>
       </c>
-      <c r="D68" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="15">
-        <v>1</v>
-      </c>
-      <c r="F68" s="15">
-        <v>1</v>
-      </c>
-      <c r="G68" s="15">
-        <v>0</v>
-      </c>
-      <c r="H68" s="15">
-        <v>0</v>
-      </c>
-      <c r="I68" s="15">
-        <v>0</v>
-      </c>
-      <c r="J68" s="15">
-        <v>0</v>
-      </c>
-      <c r="K68" s="15">
+      <c r="D68" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" s="30">
+        <v>1</v>
+      </c>
+      <c r="F68" s="30">
+        <v>1</v>
+      </c>
+      <c r="G68" s="30">
+        <v>1</v>
+      </c>
+      <c r="H68" s="30">
+        <v>1</v>
+      </c>
+      <c r="I68" s="30">
+        <v>1</v>
+      </c>
+      <c r="J68" s="30">
+        <v>1</v>
+      </c>
+      <c r="K68" s="30">
         <v>101</v>
       </c>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
+      <c r="L68" s="30">
+        <v>71</v>
+      </c>
+      <c r="M68" s="30"/>
       <c r="O68">
         <v>126</v>
       </c>
@@ -3573,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="J69" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K69" s="28"/>
       <c r="L69" s="28"/>
@@ -3615,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="J70" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70" s="28"/>
       <c r="L70" s="28"/>
@@ -3735,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="15">
         <v>0</v>
@@ -3779,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" s="15">
         <v>0</v>
@@ -3835,7 +3892,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K75" s="20"/>
       <c r="L75" s="20"/>
@@ -3879,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
@@ -4011,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="J79" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79" s="28"/>
       <c r="L79" s="28"/>
@@ -4053,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K80" s="28"/>
       <c r="L80" s="28"/>
@@ -4526,7 +4583,7 @@
         <v>22</v>
       </c>
       <c r="E91" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="15">
         <v>0</v>
@@ -4570,7 +4627,7 @@
         <v>24</v>
       </c>
       <c r="E92" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" s="15">
         <v>0</v>
@@ -4601,41 +4658,43 @@
       <c r="Q92" s="22"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A93" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B93" s="24">
+      <c r="A93" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" s="31">
         <v>28</v>
       </c>
-      <c r="C93" s="24">
+      <c r="C93" s="31">
         <v>211116</v>
       </c>
-      <c r="D93" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E93" s="15">
-        <v>0</v>
-      </c>
-      <c r="F93" s="15">
-        <v>0</v>
-      </c>
-      <c r="G93" s="15">
-        <v>0</v>
-      </c>
-      <c r="H93" s="15">
-        <v>0</v>
-      </c>
-      <c r="I93" s="15">
-        <v>0</v>
-      </c>
-      <c r="J93" s="15">
-        <v>0</v>
-      </c>
-      <c r="K93" s="15">
+      <c r="D93" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="30">
+        <v>1</v>
+      </c>
+      <c r="F93" s="30">
+        <v>1</v>
+      </c>
+      <c r="G93" s="30">
+        <v>1</v>
+      </c>
+      <c r="H93" s="30">
+        <v>1</v>
+      </c>
+      <c r="I93" s="30">
+        <v>1</v>
+      </c>
+      <c r="J93" s="30">
+        <v>1</v>
+      </c>
+      <c r="K93" s="30">
         <v>126</v>
       </c>
-      <c r="L93" s="15"/>
-      <c r="M93" s="15"/>
+      <c r="L93" s="30">
+        <v>93</v>
+      </c>
+      <c r="M93" s="30"/>
       <c r="O93">
         <v>126</v>
       </c>
@@ -4645,41 +4704,43 @@
       <c r="Q93" s="22"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" s="24">
+      <c r="A94" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" s="31">
         <v>28</v>
       </c>
-      <c r="C94" s="24">
+      <c r="C94" s="31">
         <v>211116</v>
       </c>
-      <c r="D94" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E94" s="15">
-        <v>0</v>
-      </c>
-      <c r="F94" s="15">
-        <v>0</v>
-      </c>
-      <c r="G94" s="15">
-        <v>0</v>
-      </c>
-      <c r="H94" s="15">
-        <v>0</v>
-      </c>
-      <c r="I94" s="15">
-        <v>0</v>
-      </c>
-      <c r="J94" s="15">
-        <v>0</v>
-      </c>
-      <c r="K94" s="15">
+      <c r="D94" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="30">
+        <v>1</v>
+      </c>
+      <c r="F94" s="30">
+        <v>1</v>
+      </c>
+      <c r="G94" s="30">
+        <v>1</v>
+      </c>
+      <c r="H94" s="30">
+        <v>1</v>
+      </c>
+      <c r="I94" s="30">
+        <v>1</v>
+      </c>
+      <c r="J94" s="30">
+        <v>1</v>
+      </c>
+      <c r="K94" s="30">
         <v>64</v>
       </c>
-      <c r="L94" s="15"/>
-      <c r="M94" s="15"/>
+      <c r="L94" s="30">
+        <v>51</v>
+      </c>
+      <c r="M94" s="30"/>
       <c r="O94">
         <v>78</v>
       </c>
@@ -4702,7 +4763,7 @@
         <v>22</v>
       </c>
       <c r="E95" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95" s="15">
         <v>0</v>
@@ -4746,7 +4807,7 @@
         <v>24</v>
       </c>
       <c r="E96" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="15">
         <v>0</v>
@@ -4777,41 +4838,45 @@
       <c r="Q96" s="22"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A97" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B97" s="24">
+      <c r="A97" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="31">
         <v>28</v>
       </c>
-      <c r="C97" s="24">
+      <c r="C97" s="31">
         <v>211117</v>
       </c>
-      <c r="D97" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E97" s="15">
-        <v>0</v>
-      </c>
-      <c r="F97" s="15">
-        <v>0</v>
-      </c>
-      <c r="G97" s="15">
-        <v>0</v>
-      </c>
-      <c r="H97" s="15">
-        <v>0</v>
-      </c>
-      <c r="I97" s="15">
-        <v>0</v>
-      </c>
-      <c r="J97" s="15">
-        <v>0</v>
-      </c>
-      <c r="K97" s="15">
+      <c r="D97" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" s="30">
+        <v>1</v>
+      </c>
+      <c r="F97" s="30">
+        <v>0</v>
+      </c>
+      <c r="G97" s="30">
+        <v>0</v>
+      </c>
+      <c r="H97" s="30">
+        <v>0</v>
+      </c>
+      <c r="I97" s="30">
+        <v>0</v>
+      </c>
+      <c r="J97" s="30">
+        <v>1</v>
+      </c>
+      <c r="K97" s="30">
         <v>88</v>
       </c>
-      <c r="L97" s="15"/>
-      <c r="M97" s="15"/>
+      <c r="L97" s="30">
+        <v>69</v>
+      </c>
+      <c r="M97" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="O97">
         <v>127</v>
       </c>
@@ -4820,41 +4885,45 @@
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A98" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="24">
+      <c r="A98" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="31">
         <v>28</v>
       </c>
-      <c r="C98" s="24">
+      <c r="C98" s="31">
         <v>211117</v>
       </c>
-      <c r="D98" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E98" s="15">
-        <v>0</v>
-      </c>
-      <c r="F98" s="15">
-        <v>0</v>
-      </c>
-      <c r="G98" s="15">
-        <v>0</v>
-      </c>
-      <c r="H98" s="15">
-        <v>0</v>
-      </c>
-      <c r="I98" s="15">
-        <v>0</v>
-      </c>
-      <c r="J98" s="15">
-        <v>0</v>
-      </c>
-      <c r="K98" s="15">
+      <c r="D98" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98" s="30">
+        <v>1</v>
+      </c>
+      <c r="F98" s="30">
+        <v>0</v>
+      </c>
+      <c r="G98" s="30">
+        <v>0</v>
+      </c>
+      <c r="H98" s="30">
+        <v>0</v>
+      </c>
+      <c r="I98" s="30">
+        <v>0</v>
+      </c>
+      <c r="J98" s="30">
+        <v>1</v>
+      </c>
+      <c r="K98" s="30">
         <v>131</v>
       </c>
-      <c r="L98" s="15"/>
-      <c r="M98" s="15"/>
+      <c r="L98" s="30">
+        <v>85</v>
+      </c>
+      <c r="M98" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="O98">
         <f>SUM(O53:O97)</f>
         <v>3974</v>
@@ -4877,12 +4946,24 @@
       <c r="D99" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E99" s="15"/>
-      <c r="F99" s="15"/>
-      <c r="G99" s="15"/>
-      <c r="H99" s="15"/>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
+      <c r="E99" s="15">
+        <v>1</v>
+      </c>
+      <c r="F99" s="15">
+        <v>0</v>
+      </c>
+      <c r="G99" s="15">
+        <v>0</v>
+      </c>
+      <c r="H99" s="15">
+        <v>0</v>
+      </c>
+      <c r="I99" s="15">
+        <v>0</v>
+      </c>
+      <c r="J99" s="15">
+        <v>0</v>
+      </c>
       <c r="K99" s="15">
         <v>98</v>
       </c>
@@ -4913,12 +4994,24 @@
       <c r="D100" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E100" s="15"/>
-      <c r="F100" s="15"/>
-      <c r="G100" s="15"/>
-      <c r="H100" s="15"/>
-      <c r="I100" s="15"/>
-      <c r="J100" s="15"/>
+      <c r="E100" s="15">
+        <v>1</v>
+      </c>
+      <c r="F100" s="15">
+        <v>0</v>
+      </c>
+      <c r="G100" s="15">
+        <v>0</v>
+      </c>
+      <c r="H100" s="15">
+        <v>0</v>
+      </c>
+      <c r="I100" s="15">
+        <v>0</v>
+      </c>
+      <c r="J100" s="15">
+        <v>0</v>
+      </c>
       <c r="K100" s="15">
         <v>68</v>
       </c>
@@ -4949,6 +5042,24 @@
       <c r="D101" s="24" t="s">
         <v>22</v>
       </c>
+      <c r="E101" s="15">
+        <v>1</v>
+      </c>
+      <c r="F101" s="15">
+        <v>0</v>
+      </c>
+      <c r="G101" s="15">
+        <v>0</v>
+      </c>
+      <c r="H101" s="15">
+        <v>0</v>
+      </c>
+      <c r="I101" s="15">
+        <v>0</v>
+      </c>
+      <c r="J101" s="15">
+        <v>0</v>
+      </c>
       <c r="K101" s="15">
         <v>127</v>
       </c>
@@ -4966,8 +5077,563 @@
       <c r="D102" s="24" t="s">
         <v>24</v>
       </c>
+      <c r="E102" s="15">
+        <v>1</v>
+      </c>
+      <c r="F102" s="15">
+        <v>0</v>
+      </c>
+      <c r="G102" s="15">
+        <v>0</v>
+      </c>
+      <c r="H102" s="15">
+        <v>0</v>
+      </c>
+      <c r="I102" s="15">
+        <v>0</v>
+      </c>
+      <c r="J102" s="15">
+        <v>0</v>
+      </c>
       <c r="K102" s="15">
         <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" s="21">
+        <v>28</v>
+      </c>
+      <c r="C103" s="21">
+        <v>211119</v>
+      </c>
+      <c r="D103" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E103" s="22">
+        <v>0</v>
+      </c>
+      <c r="F103" s="21">
+        <v>0</v>
+      </c>
+      <c r="G103" s="21">
+        <v>0</v>
+      </c>
+      <c r="H103" s="21">
+        <v>0</v>
+      </c>
+      <c r="I103" s="21">
+        <v>0</v>
+      </c>
+      <c r="J103" s="21">
+        <v>0</v>
+      </c>
+      <c r="K103" s="22"/>
+      <c r="L103" s="22"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A104" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" s="21">
+        <v>28</v>
+      </c>
+      <c r="C104" s="21">
+        <v>211119</v>
+      </c>
+      <c r="D104" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" s="22">
+        <v>0</v>
+      </c>
+      <c r="F104" s="21">
+        <v>0</v>
+      </c>
+      <c r="G104" s="21">
+        <v>0</v>
+      </c>
+      <c r="H104" s="21">
+        <v>0</v>
+      </c>
+      <c r="I104" s="21">
+        <v>0</v>
+      </c>
+      <c r="J104" s="21">
+        <v>0</v>
+      </c>
+      <c r="K104" s="22"/>
+      <c r="L104" s="22"/>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" s="21">
+        <v>29</v>
+      </c>
+      <c r="C105" s="21">
+        <v>211119</v>
+      </c>
+      <c r="D105" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" s="22">
+        <v>0</v>
+      </c>
+      <c r="F105" s="21">
+        <v>0</v>
+      </c>
+      <c r="G105" s="21">
+        <v>0</v>
+      </c>
+      <c r="H105" s="21">
+        <v>0</v>
+      </c>
+      <c r="I105" s="21">
+        <v>0</v>
+      </c>
+      <c r="J105" s="21">
+        <v>0</v>
+      </c>
+      <c r="K105" s="22"/>
+      <c r="L105" s="22"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" s="21">
+        <v>29</v>
+      </c>
+      <c r="C106" s="21">
+        <v>211119</v>
+      </c>
+      <c r="D106" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="22">
+        <v>0</v>
+      </c>
+      <c r="F106" s="21">
+        <v>0</v>
+      </c>
+      <c r="G106" s="21">
+        <v>0</v>
+      </c>
+      <c r="H106" s="21">
+        <v>0</v>
+      </c>
+      <c r="I106" s="21">
+        <v>0</v>
+      </c>
+      <c r="J106" s="21">
+        <v>0</v>
+      </c>
+      <c r="K106" s="22"/>
+      <c r="L106" s="22"/>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" s="21">
+        <v>28</v>
+      </c>
+      <c r="C107" s="21">
+        <v>211120</v>
+      </c>
+      <c r="D107" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E107" s="22">
+        <v>0</v>
+      </c>
+      <c r="F107" s="21">
+        <v>0</v>
+      </c>
+      <c r="G107" s="21">
+        <v>0</v>
+      </c>
+      <c r="H107" s="21">
+        <v>0</v>
+      </c>
+      <c r="I107" s="21">
+        <v>0</v>
+      </c>
+      <c r="J107" s="21">
+        <v>0</v>
+      </c>
+      <c r="K107" s="22"/>
+      <c r="L107" s="22"/>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" s="21">
+        <v>28</v>
+      </c>
+      <c r="C108" s="21">
+        <v>211120</v>
+      </c>
+      <c r="D108" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E108" s="22">
+        <v>0</v>
+      </c>
+      <c r="F108" s="21">
+        <v>0</v>
+      </c>
+      <c r="G108" s="21">
+        <v>0</v>
+      </c>
+      <c r="H108" s="21">
+        <v>0</v>
+      </c>
+      <c r="I108" s="21">
+        <v>0</v>
+      </c>
+      <c r="J108" s="21">
+        <v>0</v>
+      </c>
+      <c r="K108" s="22"/>
+      <c r="L108" s="22"/>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A109" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" s="21">
+        <v>28</v>
+      </c>
+      <c r="C109" s="21">
+        <v>211121</v>
+      </c>
+      <c r="D109" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" s="22">
+        <v>0</v>
+      </c>
+      <c r="F109" s="21">
+        <v>0</v>
+      </c>
+      <c r="G109" s="21">
+        <v>0</v>
+      </c>
+      <c r="H109" s="21">
+        <v>0</v>
+      </c>
+      <c r="I109" s="21">
+        <v>0</v>
+      </c>
+      <c r="J109" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A110" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" s="21">
+        <v>28</v>
+      </c>
+      <c r="C110" s="21">
+        <v>211121</v>
+      </c>
+      <c r="D110" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="22">
+        <v>0</v>
+      </c>
+      <c r="F110" s="21">
+        <v>0</v>
+      </c>
+      <c r="G110" s="21">
+        <v>0</v>
+      </c>
+      <c r="H110" s="21">
+        <v>0</v>
+      </c>
+      <c r="I110" s="21">
+        <v>0</v>
+      </c>
+      <c r="J110" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A111" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" s="21">
+        <v>28</v>
+      </c>
+      <c r="C111" s="21">
+        <v>211122</v>
+      </c>
+      <c r="D111" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E111" s="22">
+        <v>0</v>
+      </c>
+      <c r="F111" s="21">
+        <v>0</v>
+      </c>
+      <c r="G111" s="21">
+        <v>0</v>
+      </c>
+      <c r="H111" s="21">
+        <v>0</v>
+      </c>
+      <c r="I111" s="21">
+        <v>0</v>
+      </c>
+      <c r="J111" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A112" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" s="21">
+        <v>28</v>
+      </c>
+      <c r="C112" s="21">
+        <v>211122</v>
+      </c>
+      <c r="D112" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" s="22">
+        <v>0</v>
+      </c>
+      <c r="F112" s="21">
+        <v>0</v>
+      </c>
+      <c r="G112" s="21">
+        <v>0</v>
+      </c>
+      <c r="H112" s="21">
+        <v>0</v>
+      </c>
+      <c r="I112" s="21">
+        <v>0</v>
+      </c>
+      <c r="J112" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B113" s="21">
+        <v>29</v>
+      </c>
+      <c r="C113" s="21">
+        <v>211122</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E113" s="22">
+        <v>0</v>
+      </c>
+      <c r="F113" s="21">
+        <v>0</v>
+      </c>
+      <c r="G113" s="21">
+        <v>0</v>
+      </c>
+      <c r="H113" s="21">
+        <v>0</v>
+      </c>
+      <c r="I113" s="21">
+        <v>0</v>
+      </c>
+      <c r="J113" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" s="21">
+        <v>29</v>
+      </c>
+      <c r="C114" s="21">
+        <v>211122</v>
+      </c>
+      <c r="D114" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E114" s="22">
+        <v>0</v>
+      </c>
+      <c r="F114" s="21">
+        <v>0</v>
+      </c>
+      <c r="G114" s="21">
+        <v>0</v>
+      </c>
+      <c r="H114" s="21">
+        <v>0</v>
+      </c>
+      <c r="I114" s="21">
+        <v>0</v>
+      </c>
+      <c r="J114" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115" s="21">
+        <v>28</v>
+      </c>
+      <c r="C115" s="21">
+        <v>211123</v>
+      </c>
+      <c r="D115" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E115" s="22">
+        <v>0</v>
+      </c>
+      <c r="F115" s="21">
+        <v>0</v>
+      </c>
+      <c r="G115" s="21">
+        <v>0</v>
+      </c>
+      <c r="H115" s="21">
+        <v>0</v>
+      </c>
+      <c r="I115" s="21">
+        <v>0</v>
+      </c>
+      <c r="J115" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B116" s="21">
+        <v>28</v>
+      </c>
+      <c r="C116" s="21">
+        <v>211123</v>
+      </c>
+      <c r="D116" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E116" s="22">
+        <v>0</v>
+      </c>
+      <c r="F116" s="21">
+        <v>0</v>
+      </c>
+      <c r="G116" s="21">
+        <v>0</v>
+      </c>
+      <c r="H116" s="21">
+        <v>0</v>
+      </c>
+      <c r="I116" s="21">
+        <v>0</v>
+      </c>
+      <c r="J116" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B117" s="21">
+        <v>29</v>
+      </c>
+      <c r="C117" s="21">
+        <v>211123</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E117" s="22">
+        <v>0</v>
+      </c>
+      <c r="F117" s="21">
+        <v>0</v>
+      </c>
+      <c r="G117" s="21">
+        <v>0</v>
+      </c>
+      <c r="H117" s="21">
+        <v>0</v>
+      </c>
+      <c r="I117" s="21">
+        <v>0</v>
+      </c>
+      <c r="J117" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B118" s="21">
+        <v>29</v>
+      </c>
+      <c r="C118" s="21">
+        <v>211123</v>
+      </c>
+      <c r="D118" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E118" s="22">
+        <v>0</v>
+      </c>
+      <c r="F118" s="21">
+        <v>0</v>
+      </c>
+      <c r="G118" s="21">
+        <v>0</v>
+      </c>
+      <c r="H118" s="21">
+        <v>0</v>
+      </c>
+      <c r="I118" s="21">
+        <v>0</v>
+      </c>
+      <c r="J118" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="22"/>
+      <c r="B119" s="22"/>
+      <c r="C119" s="22"/>
+      <c r="D119" s="22"/>
+      <c r="I119" t="s">
+        <v>61</v>
+      </c>
+      <c r="J119">
+        <f>ROWS(J3:J118)-SUM(J3:J118)</f>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spike sorting progress
</commit_message>
<xml_diff>
--- a/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
+++ b/docs/metadata-summaries/UpdateTaskKilosortSummary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Teema downloaded</t>
+  </si>
+  <si>
+    <t>a messy/very split up recording but ok</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,6 +441,7 @@
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K114" sqref="K114"/>
+      <selection pane="bottomLeft" activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1116,45 +1120,49 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="16">
         <v>17</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="16">
         <v>210409</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16">
+        <v>1</v>
+      </c>
+      <c r="J8" s="16">
+        <v>1</v>
+      </c>
+      <c r="K8" s="16">
         <v>58</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="34">
+      <c r="L8" s="16">
+        <v>41</v>
+      </c>
+      <c r="M8" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="4"/>
+        <v>0.7068965517241379</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" t="s">
         <v>29</v>
@@ -1210,45 +1218,47 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="16">
         <v>17</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="16">
         <v>210410</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1</v>
+      </c>
+      <c r="J10" s="16">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16">
         <v>56</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="34">
+      <c r="L10" s="16">
+        <v>35</v>
+      </c>
+      <c r="M10" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="4" t="s">
+        <v>0.625</v>
+      </c>
+      <c r="N10" s="16" t="s">
         <v>61</v>
       </c>
       <c r="P10" s="20"/>
@@ -1390,7 +1400,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="20"/>
@@ -1434,99 +1446,101 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="16">
         <v>17</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="16">
         <v>210414</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="E15" s="16">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
+      <c r="I15" s="16">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>1</v>
+      </c>
+      <c r="K15" s="16">
         <v>67</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="34">
+      <c r="L15" s="16">
+        <v>38</v>
+      </c>
+      <c r="M15" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>0.56716417910447758</v>
+      </c>
+      <c r="N15" s="16"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="16">
         <v>17</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="16">
         <v>210414</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
+      <c r="E16" s="16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="16">
         <v>13</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="34">
+      <c r="L16" s="16">
+        <v>12</v>
+      </c>
+      <c r="M16" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="N16" s="16"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="20"/>
@@ -1632,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4">
         <v>0</v>
@@ -1654,7 +1668,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="R19" s="21"/>
     </row>
     <row r="20" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1977,45 +1993,47 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="A27" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="16">
         <v>20</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="16">
         <v>210513</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="4">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4">
-        <v>0</v>
-      </c>
-      <c r="G27" s="4">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0</v>
-      </c>
-      <c r="K27" s="4">
+      <c r="E27" s="16">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16">
+        <v>1</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1</v>
+      </c>
+      <c r="H27" s="16">
+        <v>1</v>
+      </c>
+      <c r="I27" s="16">
+        <v>1</v>
+      </c>
+      <c r="J27" s="16">
+        <v>1</v>
+      </c>
+      <c r="K27" s="16">
         <v>66</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="34">
+      <c r="L27" s="16">
+        <v>42</v>
+      </c>
+      <c r="M27" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="4"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="N27" s="16"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2899,172 +2917,176 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="4">
+      <c r="A47" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="16">
         <v>25</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="17">
         <v>210908</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="4">
-        <v>1</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0</v>
-      </c>
-      <c r="H47" s="4">
-        <v>0</v>
-      </c>
-      <c r="I47" s="4">
-        <v>0</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="4">
+      <c r="E47" s="16">
+        <v>1</v>
+      </c>
+      <c r="F47" s="16">
+        <v>1</v>
+      </c>
+      <c r="G47" s="16">
+        <v>1</v>
+      </c>
+      <c r="H47" s="16">
+        <v>1</v>
+      </c>
+      <c r="I47" s="16">
+        <v>1</v>
+      </c>
+      <c r="J47" s="16">
+        <v>1</v>
+      </c>
+      <c r="K47" s="16">
         <v>88</v>
       </c>
-      <c r="L47" s="4"/>
-      <c r="M47" s="34">
+      <c r="L47" s="16">
+        <v>69</v>
+      </c>
+      <c r="M47" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>0.78409090909090906</v>
+      </c>
+      <c r="N47" s="16"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="4">
+      <c r="A48" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="16">
         <v>25</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="17">
         <v>210908</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="4">
-        <v>1</v>
-      </c>
-      <c r="F48" s="4">
-        <v>0</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0</v>
-      </c>
-      <c r="H48" s="4">
-        <v>0</v>
-      </c>
-      <c r="I48" s="4">
-        <v>0</v>
-      </c>
-      <c r="J48" s="4">
-        <v>0</v>
-      </c>
-      <c r="K48" s="4">
+      <c r="E48" s="16">
+        <v>1</v>
+      </c>
+      <c r="F48" s="16">
+        <v>1</v>
+      </c>
+      <c r="G48" s="16">
+        <v>1</v>
+      </c>
+      <c r="H48" s="16">
+        <v>1</v>
+      </c>
+      <c r="I48" s="16">
+        <v>1</v>
+      </c>
+      <c r="J48" s="16">
+        <v>1</v>
+      </c>
+      <c r="K48" s="16">
         <v>49</v>
       </c>
-      <c r="L48" s="4"/>
-      <c r="M48" s="34">
+      <c r="L48" s="16">
+        <v>32</v>
+      </c>
+      <c r="M48" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>0.65306122448979587</v>
+      </c>
+      <c r="N48" s="16"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="4">
+      <c r="A49" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="16">
         <v>25</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="17">
         <v>210909</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="4">
-        <v>1</v>
-      </c>
-      <c r="F49" s="4">
-        <v>0</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0</v>
-      </c>
-      <c r="H49" s="4">
-        <v>0</v>
-      </c>
-      <c r="I49" s="4">
-        <v>0</v>
-      </c>
-      <c r="J49" s="4">
-        <v>0</v>
-      </c>
-      <c r="K49" s="4">
+      <c r="E49" s="16">
+        <v>1</v>
+      </c>
+      <c r="F49" s="16">
+        <v>1</v>
+      </c>
+      <c r="G49" s="16">
+        <v>1</v>
+      </c>
+      <c r="H49" s="16">
+        <v>1</v>
+      </c>
+      <c r="I49" s="16">
+        <v>1</v>
+      </c>
+      <c r="J49" s="16">
+        <v>1</v>
+      </c>
+      <c r="K49" s="16">
         <v>47</v>
       </c>
-      <c r="L49" s="4"/>
-      <c r="M49" s="34">
+      <c r="L49" s="16">
+        <v>38</v>
+      </c>
+      <c r="M49" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="4"/>
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="N49" s="16"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="4">
+      <c r="A50" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="16">
         <v>25</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="17">
         <v>210909</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="4">
-        <v>1</v>
-      </c>
-      <c r="F50" s="4">
-        <v>0</v>
-      </c>
-      <c r="G50" s="4">
-        <v>0</v>
-      </c>
-      <c r="H50" s="4">
-        <v>0</v>
-      </c>
-      <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="4">
-        <v>0</v>
-      </c>
-      <c r="K50" s="4">
+      <c r="E50" s="16">
+        <v>1</v>
+      </c>
+      <c r="F50" s="16">
+        <v>1</v>
+      </c>
+      <c r="G50" s="16">
+        <v>1</v>
+      </c>
+      <c r="H50" s="16">
+        <v>1</v>
+      </c>
+      <c r="I50" s="16">
+        <v>1</v>
+      </c>
+      <c r="J50" s="16">
+        <v>1</v>
+      </c>
+      <c r="K50" s="16">
         <v>29</v>
       </c>
-      <c r="L50" s="4"/>
-      <c r="M50" s="34">
+      <c r="L50" s="16">
+        <v>19</v>
+      </c>
+      <c r="M50" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N50" s="4"/>
+        <v>0.65517241379310343</v>
+      </c>
+      <c r="N50" s="16"/>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
@@ -5222,7 +5244,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="15">
         <v>0</v>
@@ -5322,16 +5344,16 @@
         <v>1</v>
       </c>
       <c r="F97" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97" s="28">
         <v>1</v>
@@ -5373,16 +5395,16 @@
         <v>1</v>
       </c>
       <c r="F98" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J98" s="28">
         <v>1</v>
@@ -5410,45 +5432,47 @@
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A99" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99" s="22">
+      <c r="A99" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" s="29">
         <v>28</v>
       </c>
-      <c r="C99" s="22">
+      <c r="C99" s="29">
         <v>211118</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="D99" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E99" s="15">
-        <v>1</v>
-      </c>
-      <c r="F99" s="15">
-        <v>1</v>
-      </c>
-      <c r="G99" s="15">
-        <v>0</v>
-      </c>
-      <c r="H99" s="15">
-        <v>0</v>
-      </c>
-      <c r="I99" s="15">
-        <v>0</v>
-      </c>
-      <c r="J99" s="15">
-        <v>0</v>
-      </c>
-      <c r="K99" s="15">
+      <c r="E99" s="28">
+        <v>1</v>
+      </c>
+      <c r="F99" s="28">
+        <v>1</v>
+      </c>
+      <c r="G99" s="28">
+        <v>1</v>
+      </c>
+      <c r="H99" s="28">
+        <v>1</v>
+      </c>
+      <c r="I99" s="28">
+        <v>1</v>
+      </c>
+      <c r="J99" s="28">
+        <v>1</v>
+      </c>
+      <c r="K99" s="28">
         <v>98</v>
       </c>
-      <c r="L99" s="15"/>
-      <c r="M99" s="34">
+      <c r="L99" s="28">
+        <v>63</v>
+      </c>
+      <c r="M99" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N99" s="15" t="s">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="N99" s="28" t="s">
         <v>66</v>
       </c>
       <c r="O99" s="23">
@@ -5464,45 +5488,47 @@
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B100" s="22">
+      <c r="A100" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="29">
         <v>28</v>
       </c>
-      <c r="C100" s="22">
+      <c r="C100" s="29">
         <v>211118</v>
       </c>
-      <c r="D100" s="22" t="s">
+      <c r="D100" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E100" s="15">
-        <v>1</v>
-      </c>
-      <c r="F100" s="15">
-        <v>1</v>
-      </c>
-      <c r="G100" s="15">
-        <v>0</v>
-      </c>
-      <c r="H100" s="15">
-        <v>0</v>
-      </c>
-      <c r="I100" s="15">
-        <v>0</v>
-      </c>
-      <c r="J100" s="15">
-        <v>0</v>
-      </c>
-      <c r="K100" s="15">
+      <c r="E100" s="28">
+        <v>1</v>
+      </c>
+      <c r="F100" s="28">
+        <v>1</v>
+      </c>
+      <c r="G100" s="28">
+        <v>1</v>
+      </c>
+      <c r="H100" s="28">
+        <v>1</v>
+      </c>
+      <c r="I100" s="28">
+        <v>1</v>
+      </c>
+      <c r="J100" s="28">
+        <v>1</v>
+      </c>
+      <c r="K100" s="28">
         <v>68</v>
       </c>
-      <c r="L100" s="15"/>
-      <c r="M100" s="34">
+      <c r="L100" s="28">
+        <v>47</v>
+      </c>
+      <c r="M100" s="33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N100" s="15" t="s">
+        <v>0.69117647058823528</v>
+      </c>
+      <c r="N100" s="28" t="s">
         <v>67</v>
       </c>
       <c r="O100" s="23">
@@ -5556,7 +5582,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N101" s="15"/>
+      <c r="N101" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
@@ -5597,7 +5625,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N102" s="15"/>
+      <c r="N102" s="15" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="38" t="s">
@@ -5760,82 +5790,94 @@
       <c r="N106" s="15"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A107" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B107" s="22">
+      <c r="A107" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" s="29">
         <v>28</v>
       </c>
-      <c r="C107" s="22">
+      <c r="C107" s="29">
         <v>211120</v>
       </c>
-      <c r="D107" s="22" t="s">
+      <c r="D107" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E107" s="15">
-        <v>0</v>
-      </c>
-      <c r="F107" s="22">
-        <v>0</v>
-      </c>
-      <c r="G107" s="22">
-        <v>0</v>
-      </c>
-      <c r="H107" s="22">
-        <v>0</v>
-      </c>
-      <c r="I107" s="22">
-        <v>0</v>
-      </c>
-      <c r="J107" s="22">
-        <v>0</v>
-      </c>
-      <c r="K107" s="15"/>
-      <c r="L107" s="15"/>
-      <c r="M107" s="37" t="e">
+      <c r="E107" s="28">
+        <v>1</v>
+      </c>
+      <c r="F107" s="29">
+        <v>1</v>
+      </c>
+      <c r="G107" s="29">
+        <v>1</v>
+      </c>
+      <c r="H107" s="29">
+        <v>1</v>
+      </c>
+      <c r="I107" s="29">
+        <v>1</v>
+      </c>
+      <c r="J107" s="29">
+        <v>1</v>
+      </c>
+      <c r="K107" s="28">
+        <v>72</v>
+      </c>
+      <c r="L107" s="28">
+        <v>48</v>
+      </c>
+      <c r="M107" s="40">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N107" s="15"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N107" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A108" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B108" s="22">
+      <c r="A108" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" s="29">
         <v>28</v>
       </c>
-      <c r="C108" s="22">
+      <c r="C108" s="29">
         <v>211120</v>
       </c>
-      <c r="D108" s="22" t="s">
+      <c r="D108" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E108" s="15">
-        <v>0</v>
-      </c>
-      <c r="F108" s="22">
-        <v>0</v>
-      </c>
-      <c r="G108" s="22">
-        <v>0</v>
-      </c>
-      <c r="H108" s="22">
-        <v>0</v>
-      </c>
-      <c r="I108" s="22">
-        <v>0</v>
-      </c>
-      <c r="J108" s="22">
-        <v>0</v>
-      </c>
-      <c r="K108" s="15"/>
-      <c r="L108" s="15"/>
-      <c r="M108" s="37" t="e">
+      <c r="E108" s="28">
+        <v>1</v>
+      </c>
+      <c r="F108" s="29">
+        <v>1</v>
+      </c>
+      <c r="G108" s="29">
+        <v>1</v>
+      </c>
+      <c r="H108" s="29">
+        <v>1</v>
+      </c>
+      <c r="I108" s="29">
+        <v>1</v>
+      </c>
+      <c r="J108" s="29">
+        <v>1</v>
+      </c>
+      <c r="K108" s="28">
+        <v>67</v>
+      </c>
+      <c r="L108" s="28">
+        <v>52</v>
+      </c>
+      <c r="M108" s="40">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N108" s="15"/>
+        <v>0.77611940298507465</v>
+      </c>
+      <c r="N108" s="28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
@@ -5851,7 +5893,7 @@
         <v>22</v>
       </c>
       <c r="E109" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" s="22">
         <v>0</v>
@@ -5892,7 +5934,7 @@
         <v>24</v>
       </c>
       <c r="E110" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" s="22">
         <v>0</v>
@@ -5933,7 +5975,7 @@
         <v>22</v>
       </c>
       <c r="E111" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="22">
         <v>0</v>
@@ -5972,7 +6014,7 @@
         <v>24</v>
       </c>
       <c r="E112" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" s="22">
         <v>0</v>
@@ -6089,7 +6131,7 @@
         <v>22</v>
       </c>
       <c r="E115" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" s="22">
         <v>0</v>
@@ -6128,7 +6170,7 @@
         <v>24</v>
       </c>
       <c r="E116" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" s="22">
         <v>0</v>
@@ -6241,7 +6283,7 @@
       </c>
       <c r="J119">
         <f>ROWS(J3:J118)-SUM(J3:J118)</f>
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="M119" s="35"/>
     </row>

</xml_diff>